<commit_message>
Special case delta -> inf for x = mu
</commit_message>
<xml_diff>
--- a/paper/general_xmu_bounds_approximations.xlsx
+++ b/paper/general_xmu_bounds_approximations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="50">
   <si>
     <t xml:space="preserve">x </t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cases mpmath &gt; 300 digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asymptotic_mu</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
     <numFmt numFmtId="168" formatCode="0.00%"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -227,6 +230,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -271,7 +280,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -320,10 +329,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,7 +341,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1061,15 +1082,15 @@
       <c r="D14" s="1" t="n">
         <v>0.106</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <f aca="false">B14/B13-1</f>
         <v>-0.134387351778656</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <f aca="false">C14/C13-1</f>
         <v>-0.149425287356322</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <f aca="false">D14/D13-1</f>
         <v>-0.178294573643411</v>
       </c>
@@ -1093,13 +1114,13 @@
   <dimension ref="B1:M39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,8 +1270,8 @@
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="9" t="s">
@@ -1263,7 +1284,7 @@
         <f aca="false">C10/C11</f>
         <v>0.1758</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="12" t="n">
@@ -1280,8 +1301,8 @@
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="6" t="n">
@@ -1428,8 +1449,8 @@
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="9" t="s">
@@ -1459,8 +1480,8 @@
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="9" t="s">
@@ -1490,8 +1511,8 @@
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="9" t="s">
@@ -1521,39 +1542,39 @@
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="6" t="n">
         <f aca="false">SUM(C20:C23)</f>
         <v>4868</v>
       </c>
       <c r="D24" s="10"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="6" t="s">
@@ -1592,14 +1613,14 @@
       <c r="F29" s="4" t="n">
         <v>0.00645</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>0.0284</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <f aca="false">G29/C37</f>
         <v>0.000213533834586466</v>
       </c>
-      <c r="I29" s="15" t="n">
+      <c r="I29" s="14" t="n">
         <f aca="false">H29*1000000</f>
         <v>213.533834586466</v>
       </c>
@@ -1621,18 +1642,18 @@
       <c r="F30" s="4" t="n">
         <v>8.84E-014</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>0.0016</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <f aca="false">G30/C37</f>
         <v>1.20300751879699E-005</v>
       </c>
-      <c r="I30" s="15" t="n">
+      <c r="I30" s="14" t="n">
         <f aca="false">H30*1000000</f>
         <v>12.0300751879699</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="J30" s="1" t="n">
         <f aca="false">G29/G30</f>
         <v>17.75</v>
       </c>
@@ -1799,13 +1820,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
+      <selection pane="topLeft" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.48"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1859,15 +1883,15 @@
         <v>8.402281E-011</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>2.45</v>
+        <v>2.0239</v>
       </c>
       <c r="H6" s="1" t="n">
         <f aca="false">G6/C12</f>
-        <v>0.00049</v>
+        <v>0.00040478</v>
       </c>
       <c r="I6" s="1" t="n">
         <f aca="false">H6*1000000</f>
-        <v>490</v>
+        <v>404.78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,24 +1912,24 @@
         <v>9.599432E-016</v>
       </c>
       <c r="G7" s="1" t="n">
-        <v>0.1059</v>
+        <v>0.0325</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">G7/C12</f>
-        <v>2.118E-005</v>
+        <v>6.5E-006</v>
       </c>
       <c r="I7" s="1" t="n">
         <f aca="false">H7*1000000</f>
-        <v>21.18</v>
+        <v>6.5</v>
       </c>
       <c r="J7" s="1" t="n">
         <f aca="false">G6/G7</f>
-        <v>23.1350330500472</v>
+        <v>62.2738461538461</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1"/>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>5000</v>
       </c>
     </row>
@@ -1952,13 +1976,13 @@
       <c r="F10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="16" t="n">
+      <c r="G10" s="15" t="n">
         <v>2.220446E-016</v>
       </c>
-      <c r="H10" s="16" t="n">
+      <c r="H10" s="15" t="n">
         <v>4.440892E-016</v>
       </c>
-      <c r="I10" s="16" t="n">
+      <c r="I10" s="15" t="n">
         <v>5.995204E-015</v>
       </c>
       <c r="J10" s="10"/>
@@ -1974,19 +1998,19 @@
         <f aca="false">C11/C12</f>
         <v>0.8102</v>
       </c>
-      <c r="E11" s="13" t="n">
+      <c r="E11" s="12" t="n">
         <v>0</v>
       </c>
       <c r="F11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="16" t="n">
+      <c r="G11" s="15" t="n">
         <v>2.220446E-016</v>
       </c>
-      <c r="H11" s="16" t="n">
+      <c r="H11" s="15" t="n">
         <v>5.551115E-016</v>
       </c>
-      <c r="I11" s="16" t="n">
+      <c r="I11" s="15" t="n">
         <v>2.478018E-013</v>
       </c>
       <c r="J11" s="10"/>
@@ -1996,6 +2020,316 @@
       <c r="C12" s="6" t="n">
         <f aca="false">SUM(C10:C11)</f>
         <v>5000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>3174</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <f aca="false">C17/C19</f>
+        <v>0.6348</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>4548</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <f aca="false">C18/C19</f>
+        <v>0.9096</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G20" s="8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H20" s="8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="10" t="n">
+        <v>380</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <f aca="false">C21/$C$24</f>
+        <v>0.076</v>
+      </c>
+      <c r="E21" s="17" t="n">
+        <v>5.551115E-016</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="10" t="n">
+        <v>4493</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <f aca="false">C22/$C$24</f>
+        <v>0.8986</v>
+      </c>
+      <c r="E22" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="19" t="n">
+        <v>2.22E-016</v>
+      </c>
+      <c r="G22" s="19" t="n">
+        <v>6.66E-016</v>
+      </c>
+      <c r="H22" s="15" t="n">
+        <v>5.33E-015</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="D23" s="11" t="n">
+        <f aca="false">C23/$C$24</f>
+        <v>0.0254</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="19" t="n">
+        <v>2.22E-016</v>
+      </c>
+      <c r="G23" s="19" t="n">
+        <v>4.44E-016</v>
+      </c>
+      <c r="H23" s="19" t="n">
+        <v>1.72E-015</v>
+      </c>
+      <c r="I23" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="n">
+        <f aca="false">SUM(C21:C23)</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <f aca="false">C28/C30</f>
+        <v>0.0176991150442478</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>425</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <f aca="false">C29/C30</f>
+        <v>0.940265486725664</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="0" t="n">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G31" s="8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>247</v>
+      </c>
+      <c r="D32" s="11" t="n">
+        <f aca="false">C32/$C$35</f>
+        <v>0.546460176991151</v>
+      </c>
+      <c r="E32" s="17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="18" t="n">
+        <v>3.09E-014</v>
+      </c>
+      <c r="G32" s="15" t="n">
+        <v>5.43E-014</v>
+      </c>
+      <c r="H32" s="15" t="n">
+        <v>9.6E-014</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="10" t="n">
+        <v>204</v>
+      </c>
+      <c r="D33" s="11" t="n">
+        <f aca="false">C33/$C$35</f>
+        <v>0.451327433628319</v>
+      </c>
+      <c r="E33" s="19" t="n">
+        <v>2.22E-016</v>
+      </c>
+      <c r="F33" s="19" t="n">
+        <v>1.73E-014</v>
+      </c>
+      <c r="G33" s="19" t="n">
+        <v>3.22E-014</v>
+      </c>
+      <c r="H33" s="15" t="n">
+        <v>4.73E-014</v>
+      </c>
+      <c r="I33" s="15" t="n">
+        <v>1.19E-013</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="11" t="n">
+        <f aca="false">C34/$C$35</f>
+        <v>0.00221238938053097</v>
+      </c>
+      <c r="E34" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+      <c r="F34" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+      <c r="G34" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+      <c r="H34" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+      <c r="I34" s="19" t="n">
+        <v>7.76E-013</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="0" t="n">
+        <f aca="false">SUM(C32:C34)</f>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Include performance and implementation notes
</commit_message>
<xml_diff>
--- a/paper/general_xmu_bounds_approximations.xlsx
+++ b/paper/general_xmu_bounds_approximations.xlsx
@@ -325,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -390,18 +390,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -502,16 +490,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1812,7 +1820,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <f aca="false">C11-C24</f>
         <v>132</v>
       </c>
@@ -1901,26 +1909,26 @@
       <c r="B35" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="16" t="n">
+      <c r="C35" s="10" t="n">
         <v>22</v>
       </c>
-      <c r="D35" s="17" t="n">
+      <c r="D35" s="11" t="n">
         <f aca="false">C35/$C$37</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="E35" s="18" t="n">
+      <c r="E35" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F35" s="18" t="n">
+      <c r="F35" s="12" t="n">
         <v>6.938894E-016</v>
       </c>
-      <c r="G35" s="18" t="n">
+      <c r="G35" s="12" t="n">
         <v>3.663736E-015</v>
       </c>
-      <c r="H35" s="18" t="n">
+      <c r="H35" s="12" t="n">
         <v>1.759703E-014</v>
       </c>
-      <c r="I35" s="18" t="n">
+      <c r="I35" s="12" t="n">
         <v>5.984102E-014</v>
       </c>
     </row>
@@ -1928,26 +1936,26 @@
       <c r="B36" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="16" t="n">
+      <c r="C36" s="10" t="n">
         <v>7</v>
       </c>
-      <c r="D36" s="17" t="n">
+      <c r="D36" s="11" t="n">
         <f aca="false">C36/$C$37</f>
         <v>0.053030303030303</v>
       </c>
-      <c r="E36" s="18" t="n">
+      <c r="E36" s="12" t="n">
         <v>4.440892E-016</v>
       </c>
-      <c r="F36" s="18" t="n">
+      <c r="F36" s="12" t="n">
         <v>6.106227E-016</v>
       </c>
-      <c r="G36" s="18" t="n">
+      <c r="G36" s="12" t="n">
         <v>1.998401E-015</v>
       </c>
-      <c r="H36" s="18" t="n">
+      <c r="H36" s="12" t="n">
         <v>5.394019E-013</v>
       </c>
-      <c r="I36" s="18" t="n">
+      <c r="I36" s="12" t="n">
         <v>3.217093E-012</v>
       </c>
     </row>
@@ -2131,13 +2139,13 @@
       <c r="F10" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="19" t="n">
+      <c r="G10" s="16" t="n">
         <v>2.220446E-016</v>
       </c>
-      <c r="H10" s="19" t="n">
+      <c r="H10" s="16" t="n">
         <v>4.440892E-016</v>
       </c>
-      <c r="I10" s="19" t="n">
+      <c r="I10" s="16" t="n">
         <v>5.995204E-015</v>
       </c>
       <c r="J10" s="10"/>
@@ -2159,13 +2167,13 @@
       <c r="F11" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G11" s="19" t="n">
+      <c r="G11" s="16" t="n">
         <v>2.220446E-016</v>
       </c>
-      <c r="H11" s="19" t="n">
+      <c r="H11" s="16" t="n">
         <v>5.551115E-016</v>
       </c>
-      <c r="I11" s="19" t="n">
+      <c r="I11" s="16" t="n">
         <v>2.478018E-013</v>
       </c>
       <c r="J11" s="10"/>
@@ -2282,19 +2290,19 @@
         <f aca="false">C21/$C$24</f>
         <v>0.0292436235708004</v>
       </c>
-      <c r="E21" s="19" t="n">
+      <c r="E21" s="16" t="n">
         <v>5.551115E-016</v>
       </c>
-      <c r="F21" s="20" t="n">
+      <c r="F21" s="17" t="n">
         <v>1.7E-014</v>
       </c>
-      <c r="G21" s="19" t="n">
+      <c r="G21" s="16" t="n">
         <v>2.7E-014</v>
       </c>
-      <c r="H21" s="19" t="n">
+      <c r="H21" s="16" t="n">
         <v>4.3E-014</v>
       </c>
-      <c r="I21" s="19" t="n">
+      <c r="I21" s="16" t="n">
         <v>1.15E-013</v>
       </c>
     </row>
@@ -2318,10 +2326,10 @@
       <c r="G22" s="4" t="n">
         <v>5.55E-016</v>
       </c>
-      <c r="H22" s="19" t="n">
+      <c r="H22" s="16" t="n">
         <v>3.77E-015</v>
       </c>
-      <c r="I22" s="19" t="n">
+      <c r="I22" s="16" t="n">
         <v>4.81E-013</v>
       </c>
     </row>
@@ -2466,19 +2474,19 @@
         <f aca="false">C32/$C$35</f>
         <v>0.546460176991151</v>
       </c>
-      <c r="E32" s="19" t="n">
+      <c r="E32" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F32" s="20" t="n">
+      <c r="F32" s="17" t="n">
         <v>3.09E-014</v>
       </c>
-      <c r="G32" s="19" t="n">
+      <c r="G32" s="16" t="n">
         <v>5.43E-014</v>
       </c>
-      <c r="H32" s="19" t="n">
+      <c r="H32" s="16" t="n">
         <v>9.6E-014</v>
       </c>
-      <c r="I32" s="19" t="s">
+      <c r="I32" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2502,10 +2510,10 @@
       <c r="G33" s="4" t="n">
         <v>3.22E-014</v>
       </c>
-      <c r="H33" s="19" t="n">
+      <c r="H33" s="16" t="n">
         <v>4.73E-014</v>
       </c>
-      <c r="I33" s="19" t="n">
+      <c r="I33" s="16" t="n">
         <v>1.19E-013</v>
       </c>
     </row>
@@ -2561,7 +2569,7 @@
   <dimension ref="B1:AB77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
+      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2821,50 +2829,50 @@
       <c r="D15" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="21"/>
-      <c r="C18" s="21" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
       <c r="I18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="23" t="n">
+      <c r="C19" s="20" t="n">
         <v>3135</v>
       </c>
-      <c r="D19" s="24" t="n">
+      <c r="D19" s="21" t="n">
         <f aca="false">C19/C21</f>
         <v>0.627</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23" t="n">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="n">
         <v>2.7484</v>
       </c>
-      <c r="H19" s="23" t="n">
+      <c r="H19" s="20" t="n">
         <f aca="false">G19/C21</f>
         <v>0.00054968</v>
       </c>
@@ -2874,24 +2882,24 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="23" t="n">
+      <c r="C20" s="20" t="n">
         <v>4475</v>
       </c>
-      <c r="D20" s="24" t="n">
+      <c r="D20" s="21" t="n">
         <f aca="false">C20/C21</f>
         <v>0.895</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23" t="s">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="23" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.5108</v>
       </c>
-      <c r="H20" s="23" t="n">
+      <c r="H20" s="20" t="n">
         <f aca="false">G20/C21</f>
         <v>0.00010216</v>
       </c>
@@ -2905,132 +2913,132 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="23"/>
-      <c r="C21" s="23" t="n">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20" t="n">
         <v>5000</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="25" t="n">
+      <c r="F22" s="22" t="n">
         <v>0.25</v>
       </c>
-      <c r="G22" s="25" t="n">
+      <c r="G22" s="22" t="n">
         <v>0.5</v>
       </c>
-      <c r="H22" s="25" t="n">
+      <c r="H22" s="22" t="n">
         <v>0.75</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="27" t="n">
+      <c r="C23" s="24" t="n">
         <v>5000</v>
       </c>
-      <c r="D23" s="28" t="n">
+      <c r="D23" s="25" t="n">
         <f aca="false">C23/C24</f>
         <v>1</v>
       </c>
-      <c r="E23" s="29" t="n">
+      <c r="E23" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="30" t="n">
+      <c r="F23" s="27" t="n">
         <v>2.22E-016</v>
       </c>
-      <c r="G23" s="30" t="n">
+      <c r="G23" s="27" t="n">
         <v>8.88E-016</v>
       </c>
-      <c r="H23" s="31" t="n">
+      <c r="H23" s="28" t="n">
         <v>1.09E-014</v>
       </c>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="23"/>
-      <c r="C24" s="23" t="n">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20" t="n">
         <f aca="false">SUM(C22:C23)</f>
         <v>5000</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
       <c r="L25" s="14"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="32"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
       <c r="R25" s="14"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="21"/>
-      <c r="C27" s="21" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
       <c r="N27" s="10"/>
@@ -3040,23 +3048,23 @@
       <c r="R27" s="12"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="23" t="n">
+      <c r="C28" s="20" t="n">
         <v>4</v>
       </c>
-      <c r="D28" s="24" t="n">
+      <c r="D28" s="21" t="n">
         <f aca="false">C28/C30</f>
         <v>0.00761904761904762</v>
       </c>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23" t="s">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
       <c r="K28" s="6" t="s">
         <v>55</v>
       </c>
@@ -3069,21 +3077,21 @@
       <c r="R28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="23" t="n">
+      <c r="C29" s="20" t="n">
         <v>489</v>
       </c>
-      <c r="D29" s="24" t="n">
+      <c r="D29" s="21" t="n">
         <f aca="false">C29/C30</f>
         <v>0.931428571428571</v>
       </c>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
       <c r="J29" s="6" t="s">
         <v>35</v>
       </c>
@@ -3103,16 +3111,16 @@
       <c r="R29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="23"/>
-      <c r="C30" s="23" t="n">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20" t="n">
         <v>525</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="6" t="s">
         <v>36</v>
       </c>
@@ -3132,115 +3140,115 @@
       <c r="R30" s="12"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="25" t="n">
+      <c r="F31" s="22" t="n">
         <v>0.25</v>
       </c>
-      <c r="G31" s="25" t="n">
+      <c r="G31" s="22" t="n">
         <v>0.5</v>
       </c>
-      <c r="H31" s="25" t="n">
+      <c r="H31" s="22" t="n">
         <v>0.75</v>
       </c>
-      <c r="I31" s="21" t="s">
+      <c r="I31" s="18" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="27" t="n">
+      <c r="C32" s="24" t="n">
         <v>525</v>
       </c>
-      <c r="D32" s="28" t="n">
+      <c r="D32" s="25" t="n">
         <f aca="false">C32/$C$33</f>
         <v>1</v>
       </c>
-      <c r="E32" s="30" t="n">
+      <c r="E32" s="27" t="n">
         <v>2.22E-016</v>
       </c>
-      <c r="F32" s="30" t="n">
+      <c r="F32" s="27" t="n">
         <v>2.56E-016</v>
       </c>
-      <c r="G32" s="30" t="n">
+      <c r="G32" s="27" t="n">
         <v>4.46E-014</v>
       </c>
-      <c r="H32" s="31" t="n">
+      <c r="H32" s="28" t="n">
         <v>6.99E-014</v>
       </c>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="28" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="23"/>
-      <c r="C33" s="23" t="n">
+      <c r="B33" s="20"/>
+      <c r="C33" s="20" t="n">
         <f aca="false">SUM(C32)</f>
         <v>525</v>
       </c>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="34"/>
-      <c r="C37" s="34" t="s">
+      <c r="B37" s="31"/>
+      <c r="C37" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="34" t="s">
+      <c r="B38" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="36" t="n">
+      <c r="C38" s="33" t="n">
         <v>2949</v>
       </c>
-      <c r="D38" s="37" t="n">
+      <c r="D38" s="34" t="n">
         <f aca="false">C38/C40</f>
         <v>0.68645251396648</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36" t="s">
+      <c r="E38" s="33"/>
+      <c r="F38" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G38" s="36" t="n">
+      <c r="G38" s="33" t="n">
         <v>2.7944</v>
       </c>
       <c r="H38" s="1" t="n">
@@ -3253,21 +3261,21 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="36" t="n">
+      <c r="C39" s="33" t="n">
         <v>4296</v>
       </c>
-      <c r="D39" s="37" t="n">
+      <c r="D39" s="34" t="n">
         <f aca="false">C39/C40</f>
         <v>1</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36" t="s">
+      <c r="E39" s="33"/>
+      <c r="F39" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="G39" s="36" t="n">
+      <c r="G39" s="33" t="n">
         <v>0.4403</v>
       </c>
       <c r="H39" s="1" t="n">
@@ -3284,284 +3292,292 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36" t="n">
+      <c r="B40" s="33"/>
+      <c r="C40" s="33" t="n">
         <f aca="false">C39</f>
         <v>4296</v>
       </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="38" t="n">
+      <c r="F41" s="35" t="n">
         <v>0.25</v>
       </c>
-      <c r="G41" s="38" t="n">
+      <c r="G41" s="35" t="n">
         <v>0.5</v>
       </c>
-      <c r="H41" s="38" t="n">
+      <c r="H41" s="35" t="n">
         <v>0.75</v>
       </c>
-      <c r="I41" s="34" t="s">
+      <c r="I41" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="40" t="n">
+      <c r="C42" s="37" t="n">
         <v>258</v>
       </c>
-      <c r="D42" s="41" t="n">
+      <c r="D42" s="38" t="n">
         <f aca="false">C42/$C$48</f>
         <v>0.0600558659217877</v>
       </c>
-      <c r="E42" s="42" t="n">
+      <c r="E42" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F42" s="42" t="n">
+      <c r="F42" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="G42" s="42" t="n">
+      <c r="G42" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="H42" s="42" t="s">
+      <c r="H42" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="39" t="s">
+      <c r="B43" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="40" t="n">
+      <c r="C43" s="37" t="n">
         <v>13</v>
       </c>
-      <c r="D43" s="41" t="n">
+      <c r="D43" s="38" t="n">
         <f aca="false">C43/$C$48</f>
         <v>0.00302607076350093</v>
       </c>
-      <c r="E43" s="42" t="n">
+      <c r="E43" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F43" s="42" t="n">
+      <c r="F43" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="G43" s="42" t="n">
+      <c r="G43" s="39" t="n">
         <v>8.790813E-011</v>
       </c>
-      <c r="H43" s="42" t="s">
+      <c r="H43" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I43" s="40" t="s">
+      <c r="I43" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="39" t="s">
+      <c r="B44" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="40" t="n">
+      <c r="C44" s="37" t="n">
         <v>9</v>
       </c>
-      <c r="D44" s="41" t="n">
+      <c r="D44" s="38" t="n">
         <f aca="false">C44/$C$48</f>
         <v>0.00209497206703911</v>
       </c>
-      <c r="E44" s="42" t="n">
+      <c r="E44" s="39" t="n">
         <v>2.220446E-016</v>
       </c>
-      <c r="F44" s="42" t="n">
+      <c r="F44" s="39" t="n">
         <v>1.332268E-015</v>
       </c>
-      <c r="G44" s="42" t="n">
+      <c r="G44" s="39" t="n">
         <v>2.109424E-015</v>
       </c>
-      <c r="H44" s="42" t="n">
+      <c r="H44" s="39" t="n">
         <v>7.86593E-014</v>
       </c>
-      <c r="I44" s="42" t="n">
+      <c r="I44" s="39" t="n">
         <v>6.380718E-011</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="40" t="n">
+      <c r="C45" s="37" t="n">
         <v>156</v>
       </c>
-      <c r="D45" s="41" t="n">
+      <c r="D45" s="38" t="n">
         <f aca="false">C45/$C$48</f>
         <v>0.0363128491620112</v>
       </c>
-      <c r="E45" s="42" t="n">
+      <c r="E45" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F45" s="42" t="n">
+      <c r="F45" s="39" t="n">
         <v>4.440892E-016</v>
       </c>
-      <c r="G45" s="42" t="n">
+      <c r="G45" s="39" t="n">
         <v>3.774758E-015</v>
       </c>
-      <c r="H45" s="42" t="n">
+      <c r="H45" s="39" t="n">
         <v>2.375877E-014</v>
       </c>
-      <c r="I45" s="42" t="s">
+      <c r="I45" s="39" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="39" t="s">
+      <c r="B46" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="40" t="n">
+      <c r="C46" s="37" t="n">
         <v>516</v>
       </c>
-      <c r="D46" s="41" t="n">
+      <c r="D46" s="38" t="n">
         <f aca="false">C46/$C$48</f>
         <v>0.120111731843575</v>
       </c>
-      <c r="E46" s="42" t="n">
+      <c r="E46" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F46" s="42" t="n">
+      <c r="F46" s="39" t="n">
         <v>3.330669E-016</v>
       </c>
-      <c r="G46" s="42" t="n">
+      <c r="G46" s="39" t="n">
         <v>2.220446E-015</v>
       </c>
-      <c r="H46" s="42" t="n">
+      <c r="H46" s="39" t="n">
         <v>2.070566E-013</v>
       </c>
-      <c r="I46" s="40" t="s">
+      <c r="I46" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="40" t="n">
+      <c r="C47" s="37" t="n">
         <v>3344</v>
       </c>
-      <c r="D47" s="41" t="n">
+      <c r="D47" s="38" t="n">
         <f aca="false">C47/$C$48</f>
         <v>0.778398510242086</v>
       </c>
-      <c r="E47" s="42" t="n">
+      <c r="E47" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="F47" s="42" t="n">
+      <c r="F47" s="39" t="n">
         <v>3.330669E-016</v>
       </c>
-      <c r="G47" s="42" t="n">
+      <c r="G47" s="39" t="n">
         <v>8.881784E-016</v>
       </c>
-      <c r="H47" s="42" t="n">
+      <c r="H47" s="39" t="n">
         <v>1.199041E-014</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="I47" s="37" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="36"/>
-      <c r="C48" s="36" t="n">
+      <c r="B48" s="33"/>
+      <c r="C48" s="33" t="n">
         <f aca="false">SUM(C42:C47)</f>
         <v>4296</v>
       </c>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="34" t="s">
+      <c r="B50" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
       <c r="K50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="34"/>
-      <c r="C51" s="34" t="s">
+      <c r="B51" s="31"/>
+      <c r="C51" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="K51" s="33"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="43"/>
-      <c r="N51" s="43"/>
-      <c r="O51" s="43"/>
-      <c r="P51" s="43"/>
-      <c r="Q51" s="43"/>
-      <c r="R51" s="43"/>
-      <c r="S51" s="43"/>
-      <c r="T51" s="43"/>
-      <c r="U51" s="43"/>
-      <c r="V51" s="43"/>
-      <c r="W51" s="43"/>
-      <c r="X51" s="43"/>
-      <c r="Y51" s="43"/>
-      <c r="Z51" s="43"/>
-      <c r="AA51" s="43"/>
+      <c r="D51" s="33"/>
+      <c r="E51" s="33"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="K51" s="30"/>
+      <c r="L51" s="40"/>
+      <c r="M51" s="40"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
+      <c r="T51" s="40"/>
+      <c r="U51" s="40"/>
+      <c r="V51" s="40"/>
+      <c r="W51" s="40"/>
+      <c r="X51" s="40"/>
+      <c r="Y51" s="40"/>
+      <c r="Z51" s="40"/>
+      <c r="AA51" s="40"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="36" t="n">
-        <v>73</v>
-      </c>
-      <c r="D52" s="37" t="n">
+      <c r="C52" s="33" t="n">
+        <v>70</v>
+      </c>
+      <c r="D52" s="34" t="n">
         <f aca="false">C52/C54</f>
-        <v>0.103693181818182</v>
-      </c>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36" t="s">
+        <v>0.0994318181818182</v>
+      </c>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
+      <c r="G52" s="33" t="n">
+        <v>0.1572</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <f aca="false">G52/$C$54</f>
+        <v>0.000223295454545455</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <f aca="false">H52*1000000</f>
+        <v>223.295454545455</v>
+      </c>
       <c r="K52" s="6" t="s">
         <v>55</v>
       </c>
@@ -3569,85 +3585,93 @@
       <c r="M52" s="14"/>
       <c r="N52" s="14"/>
       <c r="O52" s="14"/>
-      <c r="P52" s="32"/>
-      <c r="Q52" s="32"/>
-      <c r="R52" s="32"/>
+      <c r="P52" s="29"/>
+      <c r="Q52" s="29"/>
+      <c r="R52" s="29"/>
       <c r="S52" s="14"/>
       <c r="T52" s="14"/>
       <c r="U52" s="14"/>
       <c r="V52" s="14"/>
       <c r="W52" s="14"/>
-      <c r="X52" s="32"/>
-      <c r="Y52" s="32"/>
-      <c r="Z52" s="32"/>
+      <c r="X52" s="29"/>
+      <c r="Y52" s="29"/>
+      <c r="Z52" s="29"/>
       <c r="AA52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C53" s="36" t="n">
-        <v>415</v>
-      </c>
-      <c r="D53" s="37" t="n">
+      <c r="C53" s="33" t="n">
+        <v>409</v>
+      </c>
+      <c r="D53" s="34" t="n">
         <f aca="false">C53/C54</f>
-        <v>0.589488636363636</v>
-      </c>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36" t="s">
+        <v>0.580965909090909</v>
+      </c>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
+      <c r="G53" s="33" t="n">
+        <v>0.0668</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <f aca="false">G53/$C$54</f>
+        <v>9.48863636363636E-005</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <f aca="false">H53*1000000</f>
+        <v>94.8863636363636</v>
+      </c>
       <c r="J53" s="6" t="s">
         <v>35</v>
       </c>
       <c r="K53" s="1" t="n">
         <f aca="false">C38+C52</f>
-        <v>3022</v>
+        <v>3019</v>
       </c>
       <c r="L53" s="7" t="n">
         <f aca="false">K53/C24</f>
-        <v>0.6044</v>
-      </c>
-      <c r="M53" s="33"/>
-      <c r="N53" s="33"/>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
-      <c r="S53" s="33"/>
-      <c r="T53" s="33"/>
-      <c r="U53" s="33"/>
-      <c r="V53" s="33"/>
-      <c r="W53" s="33"/>
-      <c r="X53" s="33"/>
-      <c r="Y53" s="33"/>
-      <c r="Z53" s="33"/>
-      <c r="AA53" s="33"/>
+        <v>0.6038</v>
+      </c>
+      <c r="M53" s="30"/>
+      <c r="N53" s="30"/>
+      <c r="O53" s="30"/>
+      <c r="P53" s="30"/>
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="30"/>
+      <c r="T53" s="30"/>
+      <c r="U53" s="30"/>
+      <c r="V53" s="30"/>
+      <c r="W53" s="30"/>
+      <c r="X53" s="30"/>
+      <c r="Y53" s="30"/>
+      <c r="Z53" s="30"/>
+      <c r="AA53" s="30"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="36"/>
-      <c r="C54" s="36" t="n">
+      <c r="B54" s="33"/>
+      <c r="C54" s="33" t="n">
         <v>704</v>
       </c>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
       <c r="J54" s="6" t="s">
         <v>36</v>
       </c>
       <c r="K54" s="1" t="n">
         <f aca="false">C39+C53</f>
-        <v>4711</v>
+        <v>4705</v>
       </c>
       <c r="L54" s="7" t="n">
         <f aca="false">K54/C48</f>
-        <v>1.09660148975791</v>
+        <v>1.09520484171322</v>
       </c>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
@@ -3662,28 +3686,28 @@
       <c r="AB54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="34" t="s">
+      <c r="B55" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C55" s="34" t="s">
+      <c r="C55" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="34" t="s">
+      <c r="E55" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="F55" s="38" t="n">
+      <c r="F55" s="35" t="n">
         <v>0.25</v>
       </c>
-      <c r="G55" s="38" t="n">
+      <c r="G55" s="35" t="n">
         <v>0.5</v>
       </c>
-      <c r="H55" s="38" t="n">
+      <c r="H55" s="35" t="n">
         <v>0.75</v>
       </c>
-      <c r="I55" s="34" t="s">
+      <c r="I55" s="31" t="s">
         <v>41</v>
       </c>
       <c r="K55" s="14"/>
@@ -3698,32 +3722,32 @@
       <c r="T55" s="10"/>
       <c r="U55" s="12"/>
       <c r="V55" s="12"/>
-      <c r="AB55" s="33"/>
+      <c r="AB55" s="30"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C56" s="44" t="n">
-        <v>116</v>
-      </c>
-      <c r="D56" s="41" t="n">
+      <c r="C56" s="10" t="n">
+        <v>120</v>
+      </c>
+      <c r="D56" s="38" t="n">
         <f aca="false">C56/$C$62</f>
-        <v>0.169096209912536</v>
-      </c>
-      <c r="E56" s="45" t="n">
+        <v>0.170454545454545</v>
+      </c>
+      <c r="E56" s="12" t="n">
         <v>2.109424E-015</v>
       </c>
-      <c r="F56" s="45" t="n">
-        <v>2.299272E-013</v>
-      </c>
-      <c r="G56" s="45" t="n">
-        <v>6.300604E-010</v>
-      </c>
-      <c r="H56" s="45" t="s">
+      <c r="F56" s="12" t="n">
+        <v>3.87E-013</v>
+      </c>
+      <c r="G56" s="12" t="n">
+        <v>1.02E-009</v>
+      </c>
+      <c r="H56" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="I56" s="45" t="s">
+      <c r="I56" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K56" s="14"/>
@@ -3740,29 +3764,29 @@
       <c r="V56" s="10"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="39" t="s">
+      <c r="B57" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="44" t="n">
-        <v>13</v>
-      </c>
-      <c r="D57" s="41" t="n">
+      <c r="C57" s="10" t="n">
+        <v>14</v>
+      </c>
+      <c r="D57" s="38" t="n">
         <f aca="false">C57/$C$62</f>
-        <v>0.0189504373177843</v>
-      </c>
-      <c r="E57" s="45" t="n">
+        <v>0.0198863636363636</v>
+      </c>
+      <c r="E57" s="12" t="n">
         <v>2.664535E-015</v>
       </c>
-      <c r="F57" s="45" t="n">
-        <v>4.285461E-014</v>
-      </c>
-      <c r="G57" s="45" t="n">
-        <v>2.051692E-013</v>
-      </c>
-      <c r="H57" s="45" t="n">
-        <v>8.789769E-011</v>
-      </c>
-      <c r="I57" s="45" t="s">
+      <c r="F57" s="12" t="n">
+        <v>5.22E-014</v>
+      </c>
+      <c r="G57" s="12" t="n">
+        <v>3.65E-012</v>
+      </c>
+      <c r="H57" s="12" t="n">
+        <v>2.08E-010</v>
+      </c>
+      <c r="I57" s="12" t="s">
         <v>11</v>
       </c>
       <c r="K57" s="14"/>
@@ -3778,16 +3802,16 @@
       <c r="U57" s="10"/>
       <c r="V57" s="10"/>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="39" t="s">
+    <row r="58" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="44" t="n">
+      <c r="C58" s="43" t="n">
         <v>2</v>
       </c>
-      <c r="D58" s="41" t="n">
+      <c r="D58" s="44" t="n">
         <f aca="false">C58/$C$62</f>
-        <v>0.00291545189504373</v>
+        <v>0.00284090909090909</v>
       </c>
       <c r="E58" s="45" t="n">
         <v>9.323653E-013</v>
@@ -3804,29 +3828,30 @@
       <c r="I58" s="45" t="n">
         <v>6.380718E-011</v>
       </c>
-      <c r="K58" s="14"/>
-      <c r="L58" s="10"/>
-      <c r="M58" s="10"/>
-      <c r="N58" s="10"/>
-      <c r="O58" s="10"/>
-      <c r="P58" s="10"/>
-      <c r="Q58" s="10"/>
-      <c r="R58" s="10"/>
-      <c r="S58" s="10"/>
-      <c r="T58" s="10"/>
-      <c r="U58" s="10"/>
-      <c r="V58" s="10"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="39" t="s">
+      <c r="J58" s="46"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="43"/>
+      <c r="M58" s="43"/>
+      <c r="N58" s="43"/>
+      <c r="O58" s="43"/>
+      <c r="P58" s="43"/>
+      <c r="Q58" s="43"/>
+      <c r="R58" s="43"/>
+      <c r="S58" s="43"/>
+      <c r="T58" s="43"/>
+      <c r="U58" s="43"/>
+      <c r="V58" s="43"/>
+    </row>
+    <row r="59" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="44" t="n">
+      <c r="C59" s="43" t="n">
         <v>13</v>
       </c>
-      <c r="D59" s="41" t="n">
+      <c r="D59" s="44" t="n">
         <f aca="false">C59/$C$62</f>
-        <v>0.0189504373177843</v>
+        <v>0.0184659090909091</v>
       </c>
       <c r="E59" s="45" t="n">
         <v>2.546852E-013</v>
@@ -3843,36 +3868,37 @@
       <c r="I59" s="45" t="n">
         <v>7.961076E-011</v>
       </c>
-      <c r="N59" s="10"/>
-      <c r="O59" s="10"/>
-      <c r="P59" s="10"/>
-      <c r="Q59" s="10"/>
-      <c r="R59" s="10"/>
-      <c r="S59" s="10"/>
-      <c r="T59" s="10"/>
-      <c r="U59" s="10"/>
-      <c r="V59" s="12"/>
-      <c r="W59" s="12"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="39" t="s">
+      <c r="J59" s="46"/>
+      <c r="N59" s="43"/>
+      <c r="O59" s="43"/>
+      <c r="P59" s="43"/>
+      <c r="Q59" s="43"/>
+      <c r="R59" s="43"/>
+      <c r="S59" s="43"/>
+      <c r="T59" s="43"/>
+      <c r="U59" s="43"/>
+      <c r="V59" s="45"/>
+      <c r="W59" s="45"/>
+    </row>
+    <row r="60" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="44" t="n">
-        <v>151</v>
-      </c>
-      <c r="D60" s="41" t="n">
+      <c r="C60" s="43" t="n">
+        <v>155</v>
+      </c>
+      <c r="D60" s="44" t="n">
         <f aca="false">C60/$C$62</f>
-        <v>0.220116618075802</v>
+        <v>0.220170454545455</v>
       </c>
       <c r="E60" s="45" t="n">
         <v>9.992007E-016</v>
       </c>
       <c r="F60" s="45" t="n">
-        <v>9.831025E-013</v>
+        <v>1.11E-012</v>
       </c>
       <c r="G60" s="45" t="n">
-        <v>2.077236E-010</v>
+        <v>3.75E-010</v>
       </c>
       <c r="H60" s="45" t="s">
         <v>11</v>
@@ -3880,210 +3906,208 @@
       <c r="I60" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="N60" s="10"/>
-      <c r="O60" s="10"/>
-      <c r="P60" s="10"/>
-      <c r="Q60" s="10"/>
-      <c r="R60" s="10"/>
-      <c r="S60" s="10"/>
-      <c r="T60" s="10"/>
-      <c r="U60" s="10"/>
-      <c r="V60" s="10"/>
-      <c r="W60" s="10"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="36" t="s">
+      <c r="J60" s="46"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
+      <c r="P60" s="43"/>
+      <c r="Q60" s="43"/>
+      <c r="R60" s="43"/>
+      <c r="S60" s="43"/>
+      <c r="T60" s="43"/>
+      <c r="U60" s="43"/>
+      <c r="V60" s="43"/>
+      <c r="W60" s="43"/>
+    </row>
+    <row r="61" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C61" s="44" t="n">
-        <v>391</v>
-      </c>
-      <c r="D61" s="41" t="n">
+      <c r="C61" s="43" t="n">
+        <v>400</v>
+      </c>
+      <c r="D61" s="44" t="n">
         <f aca="false">C61/$C$62</f>
-        <v>0.56997084548105</v>
+        <v>0.568181818181818</v>
       </c>
       <c r="E61" s="45" t="n">
         <v>2.220446E-016</v>
       </c>
       <c r="F61" s="45" t="n">
-        <v>2.675637E-014</v>
+        <v>2.75E-014</v>
       </c>
       <c r="G61" s="45" t="n">
-        <v>4.707346E-014</v>
+        <v>4.76E-014</v>
       </c>
       <c r="H61" s="45" t="n">
-        <v>7.338574E-014</v>
+        <v>7.7E-014</v>
       </c>
       <c r="I61" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="N61" s="10"/>
-      <c r="O61" s="10"/>
-      <c r="P61" s="10"/>
-      <c r="Q61" s="10"/>
-      <c r="R61" s="10"/>
-      <c r="S61" s="10"/>
-      <c r="T61" s="10"/>
-      <c r="U61" s="10"/>
-      <c r="V61" s="10"/>
-      <c r="W61" s="10"/>
+      <c r="J61" s="46"/>
+      <c r="N61" s="43"/>
+      <c r="O61" s="43"/>
+      <c r="P61" s="43"/>
+      <c r="Q61" s="43"/>
+      <c r="R61" s="43"/>
+      <c r="S61" s="43"/>
+      <c r="T61" s="43"/>
+      <c r="U61" s="43"/>
+      <c r="V61" s="43"/>
+      <c r="W61" s="43"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="36"/>
-      <c r="C62" s="36" t="n">
+      <c r="B62" s="33"/>
+      <c r="C62" s="33" t="n">
         <f aca="false">SUM(C56:C61)</f>
-        <v>686</v>
-      </c>
-      <c r="D62" s="41"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
+        <v>704</v>
+      </c>
+      <c r="D62" s="38"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="1" t="n">
-        <f aca="false">C62+18</f>
-        <v>704</v>
-      </c>
-      <c r="D63" s="41"/>
+      <c r="D63" s="38"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K65" s="46"/>
-      <c r="L65" s="44"/>
-      <c r="M65" s="44"/>
-      <c r="N65" s="44"/>
-      <c r="O65" s="44"/>
-      <c r="P65" s="44"/>
-      <c r="Q65" s="44"/>
-      <c r="R65" s="44"/>
-      <c r="S65" s="44"/>
-      <c r="T65" s="44"/>
-      <c r="U65" s="45"/>
-      <c r="V65" s="45"/>
-      <c r="W65" s="45"/>
-      <c r="X65" s="45"/>
-      <c r="Y65" s="45"/>
-      <c r="Z65" s="45"/>
-      <c r="AA65" s="45"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="12"/>
+      <c r="V65" s="12"/>
+      <c r="W65" s="12"/>
+      <c r="X65" s="12"/>
+      <c r="Y65" s="12"/>
+      <c r="Z65" s="12"/>
+      <c r="AA65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K66" s="46"/>
-      <c r="L66" s="44"/>
-      <c r="M66" s="44"/>
-      <c r="N66" s="44"/>
-      <c r="O66" s="44"/>
-      <c r="P66" s="44"/>
-      <c r="Q66" s="44"/>
-      <c r="R66" s="44"/>
-      <c r="S66" s="44"/>
-      <c r="T66" s="44"/>
-      <c r="U66" s="45"/>
-      <c r="V66" s="45"/>
-      <c r="W66" s="45"/>
-      <c r="X66" s="45"/>
-      <c r="Y66" s="45"/>
-      <c r="Z66" s="45"/>
-      <c r="AA66" s="45"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
+      <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="12"/>
+      <c r="V66" s="12"/>
+      <c r="W66" s="12"/>
+      <c r="X66" s="12"/>
+      <c r="Y66" s="12"/>
+      <c r="Z66" s="12"/>
+      <c r="AA66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J67" s="2"/>
-      <c r="K67" s="46"/>
-      <c r="L67" s="44"/>
-      <c r="M67" s="44"/>
-      <c r="N67" s="44"/>
-      <c r="O67" s="44"/>
-      <c r="P67" s="44"/>
-      <c r="Q67" s="44"/>
-      <c r="R67" s="44"/>
-      <c r="S67" s="44"/>
-      <c r="T67" s="44"/>
-      <c r="U67" s="45"/>
-      <c r="V67" s="45"/>
-      <c r="W67" s="45"/>
-      <c r="X67" s="45"/>
-      <c r="Y67" s="45"/>
-      <c r="Z67" s="45"/>
-      <c r="AA67" s="45"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
+      <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="12"/>
+      <c r="V67" s="12"/>
+      <c r="W67" s="12"/>
+      <c r="X67" s="12"/>
+      <c r="Y67" s="12"/>
+      <c r="Z67" s="12"/>
+      <c r="AA67" s="12"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J68" s="2"/>
-      <c r="K68" s="46"/>
-      <c r="L68" s="44"/>
-      <c r="M68" s="44"/>
-      <c r="N68" s="44"/>
-      <c r="O68" s="44"/>
-      <c r="P68" s="44"/>
-      <c r="Q68" s="44"/>
-      <c r="R68" s="44"/>
-      <c r="S68" s="44"/>
-      <c r="T68" s="44"/>
-      <c r="U68" s="45"/>
-      <c r="V68" s="45"/>
-      <c r="W68" s="45"/>
-      <c r="X68" s="45"/>
-      <c r="Y68" s="45"/>
-      <c r="Z68" s="45"/>
-      <c r="AA68" s="45"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
+      <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="12"/>
+      <c r="V68" s="12"/>
+      <c r="W68" s="12"/>
+      <c r="X68" s="12"/>
+      <c r="Y68" s="12"/>
+      <c r="Z68" s="12"/>
+      <c r="AA68" s="12"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J69" s="33"/>
-      <c r="K69" s="46"/>
-      <c r="L69" s="44"/>
-      <c r="M69" s="44"/>
-      <c r="N69" s="44"/>
-      <c r="O69" s="44"/>
-      <c r="P69" s="44"/>
-      <c r="Q69" s="44"/>
-      <c r="R69" s="44"/>
-      <c r="S69" s="44"/>
-      <c r="T69" s="44"/>
-      <c r="U69" s="45"/>
-      <c r="V69" s="44"/>
-      <c r="W69" s="45"/>
-      <c r="X69" s="45"/>
-      <c r="Y69" s="45"/>
-      <c r="Z69" s="45"/>
-      <c r="AA69" s="45"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
+      <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="12"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="12"/>
+      <c r="X69" s="12"/>
+      <c r="Y69" s="12"/>
+      <c r="Z69" s="12"/>
+      <c r="AA69" s="12"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J70" s="33"/>
-      <c r="K70" s="46"/>
-      <c r="L70" s="44"/>
-      <c r="M70" s="44"/>
-      <c r="N70" s="44"/>
-      <c r="O70" s="44"/>
-      <c r="P70" s="44"/>
-      <c r="Q70" s="44"/>
-      <c r="R70" s="44"/>
-      <c r="S70" s="44"/>
-      <c r="T70" s="44"/>
-      <c r="U70" s="45"/>
-      <c r="V70" s="45"/>
-      <c r="W70" s="45"/>
-      <c r="X70" s="45"/>
-      <c r="Y70" s="45"/>
-      <c r="Z70" s="45"/>
-      <c r="AA70" s="45"/>
+      <c r="J70" s="30"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
+      <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="12"/>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J71" s="14"/>
-      <c r="K71" s="33"/>
-      <c r="L71" s="33"/>
-      <c r="M71" s="33"/>
-      <c r="N71" s="33"/>
-      <c r="O71" s="33"/>
-      <c r="P71" s="33"/>
-      <c r="Q71" s="33"/>
-      <c r="R71" s="33"/>
-      <c r="S71" s="33"/>
-      <c r="T71" s="33"/>
-      <c r="U71" s="33"/>
-      <c r="V71" s="33"/>
-      <c r="W71" s="33"/>
-      <c r="X71" s="33"/>
-      <c r="Y71" s="33"/>
-      <c r="Z71" s="33"/>
+      <c r="K71" s="30"/>
+      <c r="L71" s="30"/>
+      <c r="M71" s="30"/>
+      <c r="N71" s="30"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30"/>
+      <c r="Q71" s="30"/>
+      <c r="R71" s="30"/>
+      <c r="S71" s="30"/>
+      <c r="T71" s="30"/>
+      <c r="U71" s="30"/>
+      <c r="V71" s="30"/>
+      <c r="W71" s="30"/>
+      <c r="X71" s="30"/>
+      <c r="Y71" s="30"/>
+      <c r="Z71" s="30"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J72" s="14"/>

</xml_diff>

<commit_message>
Finish sections 3.1 and 3.2 after revision
</commit_message>
<xml_diff>
--- a/paper/general_xmu_bounds_approximations.xlsx
+++ b/paper/general_xmu_bounds_approximations.xlsx
@@ -325,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -490,7 +490,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -508,10 +508,6 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -2568,8 +2564,8 @@
   </sheetPr>
   <dimension ref="B1:AB77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3828,8 +3824,7 @@
       <c r="I58" s="45" t="n">
         <v>6.380718E-011</v>
       </c>
-      <c r="J58" s="46"/>
-      <c r="K58" s="47"/>
+      <c r="K58" s="46"/>
       <c r="L58" s="43"/>
       <c r="M58" s="43"/>
       <c r="N58" s="43"/>
@@ -3868,7 +3863,6 @@
       <c r="I59" s="45" t="n">
         <v>7.961076E-011</v>
       </c>
-      <c r="J59" s="46"/>
       <c r="N59" s="43"/>
       <c r="O59" s="43"/>
       <c r="P59" s="43"/>
@@ -3906,7 +3900,6 @@
       <c r="I60" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J60" s="46"/>
       <c r="N60" s="43"/>
       <c r="O60" s="43"/>
       <c r="P60" s="43"/>
@@ -3919,7 +3912,7 @@
       <c r="W60" s="43"/>
     </row>
     <row r="61" s="41" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="47" t="s">
         <v>42</v>
       </c>
       <c r="C61" s="43" t="n">
@@ -3944,7 +3937,6 @@
       <c r="I61" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="J61" s="46"/>
       <c r="N61" s="43"/>
       <c r="O61" s="43"/>
       <c r="P61" s="43"/>

</xml_diff>